<commit_message>
updated h bridge to a new one
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/matlab_and_solidworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DD13A43-C84D-4AD5-B5C6-C0C50E321C02}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D91C5B-A4F7-43F9-98DB-51ECA81E2315}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19335" yWindow="2565" windowWidth="7830" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -78,7 +78,7 @@
     <t>Distance of best</t>
   </si>
   <si>
-    <t>9.8 meters</t>
+    <t>GM8724S009 (Lab1) (lab h bridge)</t>
   </si>
 </sst>
 </file>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>5.1000000000000004E-3</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -661,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -676,11 +676,11 @@
         <v>13.37619976</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
@@ -688,7 +688,7 @@
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.25</v>
       </c>
@@ -713,14 +713,14 @@
         <v>9.1300000000000006E-2</v>
       </c>
       <c r="C21" s="5">
-        <v>290</v>
+        <v>164.02860000000001</v>
       </c>
       <c r="D21">
         <f>C21*0.10472</f>
-        <v>30.368799999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17.177074992000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.5</v>
       </c>
@@ -728,14 +728,14 @@
         <v>2.3E-2</v>
       </c>
       <c r="C22">
-        <v>361</v>
+        <v>266</v>
       </c>
       <c r="D22">
         <f>C22*0.10472</f>
-        <v>37.803919999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27.855519999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -743,14 +743,14 @@
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="C23">
-        <v>456.93090000000001</v>
+        <v>287.43610000000001</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D29" si="1">C23*0.10472</f>
-        <v>47.849803848000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D23:D27" si="1">C23*0.10472</f>
+        <v>30.100308391999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.5</v>
       </c>
@@ -758,14 +758,14 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24">
-        <v>204.67169999999999</v>
+        <v>129.08949999999999</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>21.433220423999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13.518252439999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -773,14 +773,14 @@
         <v>1.4E-2</v>
       </c>
       <c r="C25">
-        <v>202.86410000000001</v>
+        <v>140.01339999999999</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>21.243928552</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14.662203247999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2.5</v>
       </c>
@@ -788,17 +788,17 @@
         <v>9.1804823999999999E-4</v>
       </c>
       <c r="C26" s="3">
-        <v>522.51499999999999</v>
+        <v>234.69880000000001</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="1"/>
-        <v>54.717770799999997</v>
+        <v>24.577658335999999</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>3</v>
       </c>
@@ -806,14 +806,14 @@
         <v>6.38E-4</v>
       </c>
       <c r="C27" s="5">
-        <v>489.84879999999998</v>
+        <v>199.1831</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>51.296966335999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20.858454232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -821,14 +821,14 @@
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="C28" s="5">
-        <v>397.65289999999999</v>
+        <v>149.9992</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>41.642211687999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C28*0.10472</f>
+        <v>15.707916224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -836,26 +836,30 @@
         <v>2.3130905999999999E-4</v>
       </c>
       <c r="C29" s="5">
-        <v>73.196399999999997</v>
+        <v>120</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
-        <v>7.6651270079999989</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C29*0.10472</f>
+        <v>12.5664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -871,23 +875,24 @@
       <c r="E32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.25</v>
       </c>
       <c r="B33">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C33" s="5">
-        <v>315.7176</v>
+      <c r="C33">
+        <v>192.69280000000001</v>
       </c>
       <c r="D33">
-        <f>C33*0.10472</f>
-        <v>33.061947071999995</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D33:D41" si="2">C33*0.10472</f>
+        <v>20.178790016000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.5</v>
       </c>
@@ -895,14 +900,14 @@
         <v>2.3E-2</v>
       </c>
       <c r="C34">
-        <v>399.16419999999999</v>
+        <v>249.09780000000001</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D41" si="2">C34*0.10472</f>
-        <v>41.800475023999994</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>26.085521615999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -910,17 +915,20 @@
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="C35" s="3">
-        <v>561.13900000000001</v>
+        <v>330.4289</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="2"/>
-        <v>58.762476079999999</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34.602514407999998</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.5</v>
       </c>
@@ -928,14 +936,14 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C36">
-        <v>239.63650000000001</v>
+        <v>136.9496</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>25.094734280000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14.341362111999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -943,14 +951,14 @@
         <v>1.4E-2</v>
       </c>
       <c r="C37">
-        <v>259.8836</v>
+        <v>147.9128</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>27.215010591999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15.489428415999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>2.5</v>
       </c>
@@ -958,14 +966,17 @@
         <v>9.1804823999999999E-4</v>
       </c>
       <c r="C38" s="5">
-        <v>530.7654</v>
+        <v>209.69900000000001</v>
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>55.581752687999995</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21.95967928</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>3</v>
       </c>
@@ -973,14 +984,17 @@
         <v>6.38E-4</v>
       </c>
       <c r="C39" s="5">
-        <v>467.18990000000002</v>
+        <v>174.99680000000001</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>48.924126328</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18.325664895999999</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -988,14 +1002,16 @@
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="C40" s="5">
-        <v>369.40789999999998</v>
+        <v>131.25</v>
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>38.684395287999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13.744499999999999</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1003,18 +1019,21 @@
         <v>2.3130905999999999E-4</v>
       </c>
       <c r="C41" s="5">
-        <v>316.7987</v>
+        <v>105</v>
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
-        <v>33.175159864000001</v>
-      </c>
+        <v>10.9956</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A31:D31"/>
+    <mergeCell ref="G31:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented motor and h-bridge to electrical
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/matlab_and_solidworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D91C5B-A4F7-43F9-98DB-51ECA81E2315}"/>
+  <xr:revisionPtr revIDLastSave="533" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9B19BA9-DE92-4EE1-B1E9-7D3677D9CFF5}"/>
   <bookViews>
-    <workbookView xWindow="19335" yWindow="2565" windowWidth="7830" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -63,15 +63,6 @@
     <t>GM8724S009 (Lab1)</t>
   </si>
   <si>
-    <t>Nema 34 12 Nm</t>
-  </si>
-  <si>
-    <t>Nema 34 8 Nm</t>
-  </si>
-  <si>
-    <t>8.5 meters</t>
-  </si>
-  <si>
     <t>0.75 meters</t>
   </si>
   <si>
@@ -79,6 +70,54 @@
   </si>
   <si>
     <t>GM8724S009 (Lab1) (lab h bridge)</t>
+  </si>
+  <si>
+    <t>Maximum current (A)</t>
+  </si>
+  <si>
+    <t>E30-150-48 </t>
+  </si>
+  <si>
+    <t>0 (unlisted)</t>
+  </si>
+  <si>
+    <t>E30-400-48</t>
+  </si>
+  <si>
+    <t>Min supply voltage (Vm_min)</t>
+  </si>
+  <si>
+    <t>Max supply voltage (Vm_max)</t>
+  </si>
+  <si>
+    <t>Max output Voltage</t>
+  </si>
+  <si>
+    <t>Peak current (A)</t>
+  </si>
+  <si>
+    <t>Duty cycle</t>
+  </si>
+  <si>
+    <t>Current (A)</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Power (W)</t>
+  </si>
+  <si>
+    <t>at 75 degree swing</t>
+  </si>
+  <si>
+    <t>Time(s)</t>
+  </si>
+  <si>
+    <t>at start</t>
+  </si>
+  <si>
+    <t>Speed(rpm)</t>
   </si>
 </sst>
 </file>
@@ -134,18 +173,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +479,8 @@
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="30.140625" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" customWidth="1"/>
@@ -448,22 +490,25 @@
     <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2">
@@ -479,73 +524,79 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>5300</v>
+      </c>
+      <c r="E3">
+        <v>5.3</v>
+      </c>
+      <c r="F3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>5800</v>
+      </c>
+      <c r="E4">
+        <v>13.13</v>
+      </c>
+      <c r="F4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="C3">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="D3">
-        <v>1600</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>60</v>
-      </c>
-      <c r="C4">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="D4">
-        <v>1400</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.25</v>
       </c>
       <c r="B9">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>52.681399999999996</v>
       </c>
       <c r="D9">
@@ -553,7 +604,7 @@
         <v>5.5167962079999997</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -568,7 +619,7 @@
         <v>8.454684391999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -583,7 +634,7 @@
         <v>9.9986865439999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.5</v>
       </c>
@@ -598,7 +649,7 @@
         <v>4.3671276880000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -613,14 +664,14 @@
         <v>4.7739963039999997</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>2.5</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>131.02420000000001</v>
       </c>
       <c r="D14">
@@ -628,14 +679,14 @@
         <v>13.720854224</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>136.11189999999999</v>
       </c>
       <c r="D15">
@@ -643,22 +694,22 @@
         <v>14.253638167999998</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>141.19479999999999</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>14.785919455999998</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>12</v>
+      <c r="E16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -668,7 +719,7 @@
       <c r="B17" s="1">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>127.733</v>
       </c>
       <c r="D17">
@@ -678,31 +729,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -712,12 +763,12 @@
       <c r="B21">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C21" s="5">
-        <v>164.02860000000001</v>
+      <c r="C21" s="4">
+        <v>175.23859999999999</v>
       </c>
       <c r="D21">
         <f>C21*0.10472</f>
-        <v>17.177074992000001</v>
+        <v>18.350986191999997</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -728,11 +779,11 @@
         <v>2.3E-2</v>
       </c>
       <c r="C22">
-        <v>266</v>
+        <v>245.52350000000001</v>
       </c>
       <c r="D22">
-        <f>C22*0.10472</f>
-        <v>27.855519999999999</v>
+        <f t="shared" ref="D22:D29" si="1">C22*0.10472</f>
+        <v>25.711220919999999</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -743,11 +794,11 @@
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="C23">
-        <v>287.43610000000001</v>
+        <v>343.5564</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D27" si="1">C23*0.10472</f>
-        <v>30.100308391999999</v>
+        <f t="shared" si="1"/>
+        <v>35.977226207999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -758,11 +809,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24">
-        <v>129.08949999999999</v>
+        <v>135.37710000000001</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>13.518252439999998</v>
+        <v>14.176689912000001</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -773,44 +824,41 @@
         <v>1.4E-2</v>
       </c>
       <c r="C25">
-        <v>140.01339999999999</v>
+        <v>155.64519999999999</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>14.662203247999997</v>
+        <v>16.299165343999999</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26">
         <v>2.5</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C26" s="3">
-        <v>234.69880000000001</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26">
+        <v>507.51060000000001</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="1"/>
-        <v>24.577658335999999</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>11</v>
+        <v>53.146510031999995</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>3</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C27" s="5">
-        <v>199.1831</v>
+      <c r="C27" s="4">
+        <v>542.31269999999995</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>20.858454232</v>
+        <v>56.790985943999992</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -820,62 +868,62 @@
       <c r="B28" s="1">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C28" s="5">
-        <v>149.9992</v>
+      <c r="C28" s="4">
+        <v>587.13109999999995</v>
       </c>
       <c r="D28">
-        <f>C28*0.10472</f>
-        <v>15.707916224</v>
+        <f t="shared" si="1"/>
+        <v>61.484368791999991</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>5</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="3">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C29" s="5">
-        <v>120</v>
-      </c>
-      <c r="D29">
-        <f>C29*0.10472</f>
-        <v>12.5664</v>
+      <c r="C29" s="2">
+        <v>606.13789999999995</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="1"/>
+        <v>63.474760887999992</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="A31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="5"/>
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -885,11 +933,11 @@
         <v>9.1300000000000006E-2</v>
       </c>
       <c r="C33">
-        <v>192.69280000000001</v>
+        <v>208.38</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:D41" si="2">C33*0.10472</f>
-        <v>20.178790016000001</v>
+        <f>C33*0.10472</f>
+        <v>21.821553599999998</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -900,33 +948,32 @@
         <v>2.3E-2</v>
       </c>
       <c r="C34">
-        <v>249.09780000000001</v>
+        <v>292.19110000000001</v>
       </c>
       <c r="D34">
+        <f t="shared" ref="D34:D41" si="2">C34*0.10472</f>
+        <v>30.598251991999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="C35">
+        <v>407.60300000000001</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="2"/>
-        <v>26.085521615999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="C35" s="3">
-        <v>330.4289</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="2"/>
-        <v>34.602514407999998</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+        <v>42.684186159999996</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -936,11 +983,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C36">
-        <v>136.9496</v>
+        <v>160.22069999999999</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>14.341362111999999</v>
+        <v>16.778311704</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -951,48 +998,48 @@
         <v>1.4E-2</v>
       </c>
       <c r="C37">
-        <v>147.9128</v>
+        <v>184.53970000000001</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>15.489428415999999</v>
+        <v>19.324997384</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>2.5</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C38" s="5">
-        <v>209.69900000000001</v>
+      <c r="C38" s="4">
+        <v>598.10850000000005</v>
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>21.95967928</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="5"/>
+        <v>62.633922120000001</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>3</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C39" s="5">
-        <v>174.99680000000001</v>
+      <c r="C39" s="4">
+        <v>637.80650000000003</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>18.325664895999999</v>
-      </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="5"/>
+        <v>66.791096679999995</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1001,35 +1048,178 @@
       <c r="B40" s="1">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C40" s="5">
-        <v>131.25</v>
+      <c r="C40" s="4">
+        <v>683.36469999999997</v>
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>13.744499999999999</v>
+        <v>71.561951383999997</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="5"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>5</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="3">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C41" s="5">
-        <v>105</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="2">
+        <v>703.19140000000004</v>
+      </c>
+      <c r="D41" s="2">
         <f t="shared" si="2"/>
-        <v>10.9956</v>
+        <v>73.638203407999995</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="5"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>58</v>
+      </c>
+      <c r="D45">
+        <v>58</v>
+      </c>
+      <c r="E45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="B49">
+        <v>13.9939</v>
+      </c>
+      <c r="C49">
+        <v>16.636900000000001</v>
+      </c>
+      <c r="D49">
+        <v>10.3674</v>
+      </c>
+      <c r="E49">
+        <v>7.3265999999999998E-2</v>
+      </c>
+      <c r="F49">
+        <v>256.74450000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B50">
+        <v>27.9877</v>
+      </c>
+      <c r="C50">
+        <v>129.5009</v>
+      </c>
+      <c r="D50">
+        <v>18.6889</v>
+      </c>
+      <c r="E50">
+        <v>4.7229E-2</v>
+      </c>
+      <c r="F50">
+        <v>436.4015</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B51">
+        <v>41.9816</v>
+      </c>
+      <c r="C51">
+        <v>363.79410000000001</v>
+      </c>
+      <c r="D51">
+        <v>26.077100000000002</v>
+      </c>
+      <c r="E51">
+        <v>3.7272E-2</v>
+      </c>
+      <c r="F51">
+        <v>580.89430000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>55.9754</v>
+      </c>
+      <c r="C52">
+        <v>724.96600000000001</v>
+      </c>
+      <c r="D52">
+        <v>32.876300000000001</v>
+      </c>
+      <c r="E52">
+        <v>3.1528E-2</v>
+      </c>
+      <c r="F52">
+        <v>703.19140000000004</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="C47:F47"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A31:D31"/>

</xml_diff>

<commit_message>
New motor QBL5704-116-04-042, max distance ~ 5 meters
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/matlab_and_solidworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="533" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9B19BA9-DE92-4EE1-B1E9-7D3677D9CFF5}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC1D6B81-7BA1-40BE-94D2-6CC0B157201D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -63,12 +63,6 @@
     <t>GM8724S009 (Lab1)</t>
   </si>
   <si>
-    <t>0.75 meters</t>
-  </si>
-  <si>
-    <t>Distance of best</t>
-  </si>
-  <si>
     <t>GM8724S009 (Lab1) (lab h bridge)</t>
   </si>
   <si>
@@ -118,6 +112,9 @@
   </si>
   <si>
     <t>Speed(rpm)</t>
+  </si>
+  <si>
+    <t>QBL5704-116-04-042</t>
   </si>
 </sst>
 </file>
@@ -183,10 +180,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -526,13 +523,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>5300</v>
@@ -546,13 +543,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>5800</v>
@@ -564,13 +561,33 @@
         <v>280</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D5">
+        <v>5500</v>
+      </c>
+      <c r="E5">
+        <v>1.3</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -585,9 +602,7 @@
       <c r="D8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -708,9 +723,6 @@
         <f t="shared" si="0"/>
         <v>14.785919455999998</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -732,12 +744,12 @@
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -752,9 +764,7 @@
       <c r="D20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -896,16 +906,16 @@
       <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="A31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -920,9 +930,7 @@
       <c r="D32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E32" s="6"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1077,16 +1085,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1105,35 +1113,35 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="10"/>
+      <c r="C47" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="G48" s="6"/>
     </row>

</xml_diff>

<commit_message>
made simulink model more clear and updated some parameters
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/matlab_and_solidworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/mse312_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="546" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC1D6B81-7BA1-40BE-94D2-6CC0B157201D}"/>
+  <xr:revisionPtr revIDLastSave="566" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFC923D3-77F1-47E6-A2AC-AF96D8D02033}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="3195" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>QBL5704-116-04-042</t>
+  </si>
+  <si>
+    <t>rotor damping (N*m*s)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,9 +479,8 @@
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="30.140625" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
@@ -487,7 +489,7 @@
     <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
@@ -495,16 +497,19 @@
         <v>4</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -515,73 +520,85 @@
         <v>2.3400000000000001E-3</v>
       </c>
       <c r="D2">
+        <v>0.3</v>
+      </c>
+      <c r="E2">
         <v>720</v>
       </c>
-      <c r="E2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>1.3999999999999999E-6</v>
+      </c>
+      <c r="G2">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>1.3</v>
+      </c>
+      <c r="E3">
+        <v>5500</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G3">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>5300</v>
-      </c>
-      <c r="E3">
-        <v>5.3</v>
-      </c>
-      <c r="F3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B4">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D4">
+        <v>13.13</v>
+      </c>
+      <c r="E4">
+        <v>5800</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="G4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>5800</v>
-      </c>
-      <c r="E4">
-        <v>13.13</v>
-      </c>
-      <c r="F4">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1E-3</v>
-      </c>
       <c r="D5">
-        <v>5500</v>
+        <v>5.3</v>
       </c>
       <c r="E5">
-        <v>1.3</v>
-      </c>
-      <c r="F5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5300</v>
+      </c>
+      <c r="G5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
@@ -589,7 +606,7 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -603,8 +620,9 @@
         <v>2</v>
       </c>
       <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.25</v>
       </c>
@@ -619,7 +637,7 @@
         <v>5.5167962079999997</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -634,7 +652,7 @@
         <v>8.454684391999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -649,7 +667,7 @@
         <v>9.9986865439999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.5</v>
       </c>
@@ -664,7 +682,7 @@
         <v>4.3671276880000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -679,7 +697,7 @@
         <v>4.7739963039999997</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2.5</v>
       </c>
@@ -694,7 +712,7 @@
         <v>13.720854224</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>3</v>
       </c>
@@ -709,7 +727,7 @@
         <v>14.253638167999998</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -765,6 +783,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -912,7 +931,6 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
-      <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
@@ -931,6 +949,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -977,7 +996,6 @@
         <f t="shared" si="2"/>
         <v>42.684186159999996</v>
       </c>
-      <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -1027,7 +1045,6 @@
         <f t="shared" si="2"/>
         <v>62.633922120000001</v>
       </c>
-      <c r="G38" s="4"/>
       <c r="H38" s="5"/>
       <c r="I38" s="4"/>
     </row>
@@ -1045,7 +1062,6 @@
         <f t="shared" si="2"/>
         <v>66.791096679999995</v>
       </c>
-      <c r="G39" s="4"/>
       <c r="H39" s="5"/>
       <c r="I39" s="4"/>
     </row>
@@ -1096,6 +1112,7 @@
       <c r="E44" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -1122,7 +1139,7 @@
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="9"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -1140,12 +1157,12 @@
       <c r="E48" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="6"/>
+      <c r="G48" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>0.25</v>
       </c>
@@ -1161,11 +1178,11 @@
       <c r="E49">
         <v>7.3265999999999998E-2</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>256.74450000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>0.5</v>
       </c>
@@ -1181,11 +1198,11 @@
       <c r="E50">
         <v>4.7229E-2</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>436.4015</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>0.75</v>
       </c>
@@ -1201,11 +1218,11 @@
       <c r="E51">
         <v>3.7272E-2</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>580.89430000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1</v>
       </c>
@@ -1221,17 +1238,17 @@
       <c r="E52">
         <v>3.1528E-2</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>703.19140000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C47:G47"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="H31:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated excel table for motor specs
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/mse312_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="566" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFC923D3-77F1-47E6-A2AC-AF96D8D02033}"/>
+  <xr:revisionPtr revIDLastSave="614" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BCF8EBD-7911-4F63-AAAB-5B512F5DCBC0}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3195" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -72,9 +72,6 @@
     <t>E30-150-48 </t>
   </si>
   <si>
-    <t>0 (unlisted)</t>
-  </si>
-  <si>
     <t>E30-400-48</t>
   </si>
   <si>
@@ -117,14 +114,23 @@
     <t>QBL5704-116-04-042</t>
   </si>
   <si>
-    <t>rotor damping (N*m*s)</t>
+    <t>Internal Gear Ratio</t>
+  </si>
+  <si>
+    <t>Torque Constant (N-m/A)</t>
+  </si>
+  <si>
+    <t>Rotor Inertia kg-m^2</t>
+  </si>
+  <si>
+    <t>rotor damping (N-m-s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +145,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -161,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,11 +188,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -186,6 +220,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,775 +523,837 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="7" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2">
+        <v>2.3400000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>720</v>
+      </c>
+      <c r="E2">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>2.3400000000000001E-3</v>
-      </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
-      <c r="E2">
-        <v>720</v>
-      </c>
       <c r="F2" s="1">
+        <v>1.5999999999999999E-6</v>
+      </c>
+      <c r="G2" s="1">
         <v>1.3999999999999999E-6</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="I2">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C3">
+        <v>1.3</v>
+      </c>
+      <c r="D3">
+        <v>5500</v>
+      </c>
+      <c r="E3">
         <v>36</v>
       </c>
-      <c r="C3" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="D3">
-        <v>1.3</v>
-      </c>
-      <c r="E3">
-        <v>5500</v>
-      </c>
       <c r="F3" s="1">
+        <v>2.3E-5</v>
+      </c>
+      <c r="G3" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>5.3</v>
+      </c>
+      <c r="D4">
+        <v>5600</v>
+      </c>
+      <c r="E4">
         <v>45</v>
       </c>
-      <c r="C4" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="D4">
+      <c r="F4" s="1">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.5E-6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I4">
+        <v>70</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8.0500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="C6">
         <v>13.13</v>
       </c>
-      <c r="E4">
+      <c r="D6">
         <v>5800</v>
       </c>
-      <c r="F4" s="1">
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="G6" s="1">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="G4">
+      <c r="H6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I6">
         <v>280</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>5.3</v>
-      </c>
-      <c r="E5">
-        <v>5300</v>
-      </c>
-      <c r="G5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="J6" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>0.25</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>52.681399999999996</v>
       </c>
-      <c r="D9">
-        <f>C9*0.10472</f>
+      <c r="D10">
+        <f>C10*0.10472</f>
         <v>5.5167962079999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>0.5</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>2.3E-2</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>80.736099999999993</v>
       </c>
-      <c r="D10">
-        <f t="shared" ref="D10:D17" si="0">C10*0.10472</f>
+      <c r="D11">
+        <f t="shared" ref="D11:D18" si="0">C11*0.10472</f>
         <v>8.454684391999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>95.480199999999996</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>9.9986865439999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>1.5</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>41.7029</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>4.3671276880000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>1.4E-2</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>45.588200000000001</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>4.7739963039999997</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>2.5</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C15" s="4">
         <v>131.02420000000001</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>13.720854224</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B16" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C16" s="4">
         <v>136.11189999999999</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>14.253638167999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>4</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>141.19479999999999</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>14.785919455999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>5</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>127.733</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>13.37619976</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="4"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>0.25</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C22" s="4">
         <v>175.23859999999999</v>
       </c>
-      <c r="D21">
-        <f>C21*0.10472</f>
+      <c r="D22">
+        <f>C22*0.10472</f>
         <v>18.350986191999997</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>0.5</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>2.3E-2</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>245.52350000000001</v>
       </c>
-      <c r="D22">
-        <f t="shared" ref="D22:D29" si="1">C22*0.10472</f>
+      <c r="D23">
+        <f t="shared" ref="D23:D30" si="1">C23*0.10472</f>
         <v>25.711220919999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>343.5564</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <f t="shared" si="1"/>
         <v>35.977226207999998</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1.5</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>135.37710000000001</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f t="shared" si="1"/>
         <v>14.176689912000001</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>2</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>1.4E-2</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>155.64519999999999</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f t="shared" si="1"/>
         <v>16.299165343999999</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>2.5</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B27" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>507.51060000000001</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f t="shared" si="1"/>
         <v>53.146510031999995</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>3</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B28" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C28" s="4">
         <v>542.31269999999995</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f t="shared" si="1"/>
         <v>56.790985943999992</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>4</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="1">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C29" s="4">
         <v>587.13109999999995</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f t="shared" si="1"/>
         <v>61.484368791999991</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>5</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B30" s="3">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <v>606.13789999999995</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <f t="shared" si="1"/>
         <v>63.474760887999992</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>0.25</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>208.38</v>
       </c>
-      <c r="D33">
-        <f>C33*0.10472</f>
+      <c r="D34">
+        <f>C34*0.10472</f>
         <v>21.821553599999998</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>0.5</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>2.3E-2</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>292.19110000000001</v>
       </c>
-      <c r="D34">
-        <f t="shared" ref="D34:D41" si="2">C34*0.10472</f>
+      <c r="D35">
+        <f t="shared" ref="D35:D42" si="2">C35*0.10472</f>
         <v>30.598251991999998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>1</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>407.60300000000001</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f t="shared" si="2"/>
         <v>42.684186159999996</v>
       </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>1.5</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>160.22069999999999</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <f t="shared" si="2"/>
         <v>16.778311704</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>2</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>1.4E-2</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>184.53970000000001</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <f t="shared" si="2"/>
         <v>19.324997384</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>2.5</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B39" s="5">
         <v>9.1804823999999999E-4</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C39" s="4">
         <v>598.10850000000005</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f t="shared" si="2"/>
         <v>62.633922120000001</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="I39" s="5"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>3</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B40" s="5">
         <v>6.38E-4</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C40" s="4">
         <v>637.80650000000003</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f t="shared" si="2"/>
         <v>66.791096679999995</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="I40" s="5"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>4</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B41" s="1">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C41" s="4">
         <v>683.36469999999997</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <f t="shared" si="2"/>
         <v>71.561951383999997</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="I41" s="1"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>5</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="3">
         <v>2.3130905999999999E-4</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C42" s="2">
         <v>703.19140000000004</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D42" s="2">
         <f t="shared" si="2"/>
         <v>73.638203407999995</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
+      <c r="I42" s="1"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>58</v>
+      </c>
+      <c r="D46">
+        <v>58</v>
+      </c>
+      <c r="E46">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>7</v>
-      </c>
-      <c r="C45">
-        <v>58</v>
-      </c>
-      <c r="D45">
-        <v>58</v>
-      </c>
-      <c r="E45">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="9" t="s">
+      <c r="B49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <v>0.25</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>13.9939</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>16.636900000000001</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>10.3674</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>7.3265999999999998E-2</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>256.74450000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>0.5</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>27.9877</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>129.5009</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>18.6889</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>4.7229E-2</v>
       </c>
-      <c r="G50">
+      <c r="G51">
         <v>436.4015</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>0.75</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>41.9816</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>363.79410000000001</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <v>26.077100000000002</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>3.7272E-2</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>580.89430000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>1</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>55.9754</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>724.96600000000001</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>32.876300000000001</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <v>3.1528E-2</v>
       </c>
-      <c r="G52">
+      <c r="G53">
         <v>703.19140000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="I32:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new motor 2, updated control parameters
</commit_message>
<xml_diff>
--- a/motor_results.xlsx
+++ b/motor_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/mse312_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="635" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4796360-6F7F-4E35-A6A8-4917F2D7137B}"/>
+  <xr:revisionPtr revIDLastSave="668" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7312A3DD-A656-4CAC-B026-77C0C9E93435}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="2445" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14865" yWindow="2640" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Gear Ratio</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>armature resistance (Ohms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crouzet 82890	</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -156,6 +159,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,38 +533,38 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>11</v>
+      <c r="A3" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1">
-        <v>3.5000000000000001E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="C3">
-        <v>5.3</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>5600</v>
+        <v>3700</v>
       </c>
       <c r="E3">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
-        <v>3.4999999999999997E-5</v>
+        <v>7.9499999999999994E-5</v>
       </c>
       <c r="G3" s="1">
         <v>1.5E-6</v>
       </c>
       <c r="H3" s="1">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="I3">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1">
-        <v>8.0500000000000002E-2</v>
+        <v>34.1</v>
       </c>
       <c r="K3">
-        <v>0.70799999999999996</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>